<commit_message>
clarify status report for unit tests
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Bonds.xlsx
+++ b/UnitTests/Tests/Bonds.xlsx
@@ -644,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(B3=C3,"PASS","FAIL")</f>
+        <f>IF(ISERROR(B3),"ERROR",IF(ISERROR(C3),"FAIL",IF(B3=C3,"PASS","FAIL")))</f>
         <v>FAIL</v>
       </c>
       <c r="E3">
@@ -660,7 +660,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D54" si="0">IF(B4=C4,"PASS","FAIL")</f>
+        <f t="shared" ref="D4:D54" si="0">IF(ISERROR(B4),"ERROR",IF(ISERROR(C4),"FAIL",IF(B4=C4,"PASS","FAIL")))</f>
         <v>FAIL</v>
       </c>
       <c r="E4" t="str">
@@ -1303,9 +1303,9 @@
       <c r="B44" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="D44" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
       </c>
       <c r="E44" t="e">
         <f>_xll.qlBondSetCouponPricer()</f>
@@ -1319,9 +1319,9 @@
       <c r="B45" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="D45" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
       </c>
       <c r="E45" t="e">
         <f>_xll.qlBondSetCouponPricers()</f>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="K46" t="str">
         <f>_xll.qlInterestRate(,1,"actual/360","simple","annual")</f>
-        <v>obj_00001#0000</v>
+        <v>obj_00003#0000</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="K47" t="str">
         <f>_xll.qlInterestRate(,2,"actual/360","simple","annual")</f>
-        <v>obj_00004#0000</v>
+        <v>obj_00002#0000</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="G48" t="str">
         <f>_xll.qlIborIndex(,"euribor","1d",2,"eur","target","mf",TRUE,"actual/360")</f>
-        <v>obj_00003#0000</v>
+        <v>obj_00004#0000</v>
       </c>
       <c r="I48" s="4">
         <f t="shared" si="1"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="K48" t="str">
         <f>_xll.qlInterestRate(,3,"actual/360","simple","annual")</f>
-        <v>obj_00002#0000</v>
+        <v>obj_00001#0000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="G51" t="str">
         <f>_xll.qlLeg(,J46:J48,I46:I48)</f>
-        <v>obj_0000c#0000</v>
+        <v>obj_00008#0000</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1484,9 +1484,9 @@
       <c r="B52" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D52" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ERROR</v>
       </c>
       <c r="E52" t="e">
         <f>_xll.qlBondAlive(E51,I47)</f>

</xml_diff>

<commit_message>
export bond functions to excel (584/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Bonds.xlsx
+++ b/UnitTests/Tests/Bonds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Function</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>bond06</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
       </c>
       <c r="G27" t="str">
         <f>_xll.qlFlatForward(,0,"target",1,"actual/360","simple","annual")</f>
-        <v>obj_00000#0000</v>
+        <v>obj_00003#0000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1360,7 +1363,7 @@
       </c>
       <c r="K46" t="str">
         <f>_xll.qlInterestRate(,1,"actual/360","simple","annual")</f>
-        <v>obj_00003#0000</v>
+        <v>obj_00001#0000</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1387,7 +1390,7 @@
       </c>
       <c r="K47" t="str">
         <f>_xll.qlInterestRate(,2,"actual/360","simple","annual")</f>
-        <v>obj_00002#0000</v>
+        <v>obj_00004#0000</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,7 +1410,7 @@
       </c>
       <c r="G48" t="str">
         <f>_xll.qlIborIndex(,"euribor","1d",2,"eur","target","mf",TRUE,"actual/360")</f>
-        <v>obj_00004#0000</v>
+        <v>obj_00002#0000</v>
       </c>
       <c r="I48" s="4">
         <f t="shared" si="1"/>
@@ -1418,7 +1421,7 @@
       </c>
       <c r="K48" t="str">
         <f>_xll.qlInterestRate(,3,"actual/360","simple","annual")</f>
-        <v>obj_00001#0000</v>
+        <v>obj_00000#0000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,7 +1477,7 @@
       </c>
       <c r="G51" t="str">
         <f>_xll.qlLeg(,J46:J48,I46:I48)</f>
-        <v>obj_00008#0000</v>
+        <v>obj_00009#0000</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1496,6 +1499,9 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
export to excel the functions using type InterestRate, plus a couple other functions that got left behind (701/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Bonds.xlsx
+++ b/UnitTests/Tests/Bonds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Function</t>
   </si>
@@ -213,28 +213,10 @@
     <t>Payment Date</t>
   </si>
   <si>
-    <t>bond01#0000</t>
-  </si>
-  <si>
-    <t>bond02#0000</t>
-  </si>
-  <si>
-    <t>bond03#0000</t>
-  </si>
-  <si>
-    <t>bond04#0000</t>
-  </si>
-  <si>
-    <t>bond05#0000</t>
-  </si>
-  <si>
-    <t>bond06#0000</t>
-  </si>
-  <si>
-    <t>bond06</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t>obj_0000c</t>
   </si>
 </sst>
 </file>
@@ -651,7 +633,7 @@
         <v>FAIL</v>
       </c>
       <c r="E3">
-        <f>_xll.qlBondSettlementDays(E51)</f>
+        <f>_xll.qlBondSettlementDays(F51)</f>
         <v>2</v>
       </c>
     </row>
@@ -667,7 +649,7 @@
         <v>FAIL</v>
       </c>
       <c r="E4" t="str">
-        <f>_xll.qlBondCalendar(E51)</f>
+        <f>_xll.qlBondCalendar(F51)</f>
         <v>TARGET</v>
       </c>
     </row>
@@ -683,7 +665,7 @@
         <v>FAIL</v>
       </c>
       <c r="E5">
-        <f>_xll.qlBondNotionals(E51)</f>
+        <f>_xll.qlBondNotionals(F51)</f>
         <v>100</v>
       </c>
     </row>
@@ -699,7 +681,7 @@
         <v>PASS</v>
       </c>
       <c r="E6">
-        <f>_xll.qlBondNotional(E51)</f>
+        <f>_xll.qlBondNotional(F51)</f>
         <v>0</v>
       </c>
     </row>
@@ -715,7 +697,7 @@
         <v>FAIL</v>
       </c>
       <c r="E7">
-        <f>_xll.qlBondMaturityDate(E51)</f>
+        <f>_xll.qlBondMaturityDate(F51)</f>
         <v>42647</v>
       </c>
     </row>
@@ -731,7 +713,7 @@
         <v>FAIL</v>
       </c>
       <c r="E8">
-        <f>_xll.qlBondIssueDate(E51)</f>
+        <f>_xll.qlBondIssueDate(F51)</f>
         <v>42644</v>
       </c>
     </row>
@@ -747,7 +729,7 @@
         <v>PASS</v>
       </c>
       <c r="E9" t="b">
-        <f>_xll.qlBondIsTradable(E51)</f>
+        <f>_xll.qlBondIsTradable(F51)</f>
         <v>0</v>
       </c>
     </row>
@@ -763,7 +745,7 @@
         <v>FAIL</v>
       </c>
       <c r="E10">
-        <f>_xll.qlBondSettlementDate(E51)</f>
+        <f>_xll.qlBondSettlementDate(F51)</f>
         <v>42647</v>
       </c>
     </row>
@@ -779,7 +761,7 @@
         <v>FAIL</v>
       </c>
       <c r="E11">
-        <f>_xll.qlBondStartDate(E51)</f>
+        <f>_xll.qlBondStartDate(F51)</f>
         <v>42645</v>
       </c>
     </row>
@@ -795,7 +777,7 @@
         <v>FAIL</v>
       </c>
       <c r="E12">
-        <f>_xll.qlBondPreviousCashFlowDate(E51)</f>
+        <f>_xll.qlBondPreviousCashFlowDate(F51)</f>
         <v>42647</v>
       </c>
     </row>
@@ -811,7 +793,7 @@
         <v>PASS</v>
       </c>
       <c r="E13">
-        <f>_xll.qlBondNextCashFlowDate(E51)</f>
+        <f>_xll.qlBondNextCashFlowDate(F51)</f>
         <v>0</v>
       </c>
     </row>
@@ -827,7 +809,7 @@
         <v>FAIL</v>
       </c>
       <c r="E14">
-        <f>_xll.qlBondPreviousCashFlowAmount(E51)</f>
+        <f>_xll.qlBondPreviousCashFlowAmount(F51)</f>
         <v>3</v>
       </c>
     </row>
@@ -843,7 +825,7 @@
         <v>PASS</v>
       </c>
       <c r="E15">
-        <f>_xll.qlBondNextCashFlowAmount(E51)</f>
+        <f>_xll.qlBondNextCashFlowAmount(F51)</f>
         <v>0</v>
       </c>
     </row>
@@ -859,7 +841,7 @@
         <v>FAIL</v>
       </c>
       <c r="E16">
-        <f>_xll.qlBondPreviousCouponRate(E47)</f>
+        <f>_xll.qlBondPreviousCouponRate(F47)</f>
         <v>3</v>
       </c>
     </row>
@@ -875,7 +857,7 @@
         <v>PASS</v>
       </c>
       <c r="E17">
-        <f>_xll.qlBondNextCouponRate(E47)</f>
+        <f>_xll.qlBondNextCouponRate(F47)</f>
         <v>0</v>
       </c>
     </row>
@@ -891,7 +873,7 @@
         <v>PASS</v>
       </c>
       <c r="E18">
-        <f>_xll.qlBondAccrualStartDate(E51,I47)</f>
+        <f>_xll.qlBondAccrualStartDate(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -907,7 +889,7 @@
         <v>PASS</v>
       </c>
       <c r="E19">
-        <f>_xll.qlBondAccrualEndDate(E51,I47)</f>
+        <f>_xll.qlBondAccrualEndDate(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -923,7 +905,7 @@
         <v>PASS</v>
       </c>
       <c r="E20">
-        <f>_xll.qlBondReferencePeriodStart(E51,I47)</f>
+        <f>_xll.qlBondReferencePeriodStart(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -939,7 +921,7 @@
         <v>PASS</v>
       </c>
       <c r="E21">
-        <f>_xll.qlBondReferencePeriodEnd(E51,I47)</f>
+        <f>_xll.qlBondReferencePeriodEnd(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -955,7 +937,7 @@
         <v>PASS</v>
       </c>
       <c r="E22">
-        <f>_xll.qlBondAccrualPeriod(E51,I47)</f>
+        <f>_xll.qlBondAccrualPeriod(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -971,7 +953,7 @@
         <v>PASS</v>
       </c>
       <c r="E23">
-        <f>_xll.qlBondAccrualDays(E51,I47)</f>
+        <f>_xll.qlBondAccrualDays(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -987,7 +969,7 @@
         <v>PASS</v>
       </c>
       <c r="E24">
-        <f>_xll.qlBondAccruedPeriod(E51,I47)</f>
+        <f>_xll.qlBondAccruedPeriod(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -1003,7 +985,7 @@
         <v>PASS</v>
       </c>
       <c r="E25">
-        <f>_xll.qlBondAccruedDays(E51,I47)</f>
+        <f>_xll.qlBondAccruedDays(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -1019,7 +1001,7 @@
         <v>PASS</v>
       </c>
       <c r="E26">
-        <f>_xll.qlBondAccruedAmount(E51,I47)</f>
+        <f>_xll.qlBondAccruedAmount(F51,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -1035,12 +1017,12 @@
         <v>FAIL</v>
       </c>
       <c r="E27">
-        <f>_xll.qlBondCleanPriceFromYieldTermStructure(E51,G27,I47)</f>
+        <f>_xll.qlBondCleanPriceFromYieldTermStructure(F51,G27,I47)</f>
         <v>2.9916897506925206</v>
       </c>
       <c r="G27" t="str">
         <f>_xll.qlFlatForward(,0,"target",1,"actual/360","simple","annual")</f>
-        <v>obj_00003#0000</v>
+        <v>obj_00002#0002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,7 +1037,7 @@
         <v>PASS</v>
       </c>
       <c r="E28">
-        <f>_xll.qlBondBpsFromYieldTermStructure(E51,G27,I47)</f>
+        <f>_xll.qlBondBpsFromYieldTermStructure(F51,G27,I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1053,7 @@
         <v>FAIL</v>
       </c>
       <c r="E29">
-        <f>_xll.qlBondAtmRateFromYieldTermStructure(E47,G27,I47,100)</f>
+        <f>_xll.qlBondAtmRateFromYieldTermStructure(F47,G27,I47,100)</f>
         <v>0.99999999999997435</v>
       </c>
     </row>
@@ -1087,7 +1069,7 @@
         <v>FAIL</v>
       </c>
       <c r="E30">
-        <f>_xll.qlBondCleanPriceFromYield(E51,1,"actual/360","simple","annual",I47)</f>
+        <f>_xll.qlBondCleanPriceFromYield(F51,1,"actual/360","simple","annual",I47)</f>
         <v>2.9916897506925206</v>
       </c>
     </row>
@@ -1103,7 +1085,7 @@
         <v>FAIL</v>
       </c>
       <c r="E31">
-        <f>_xll.qlBondDirtyPriceFromYield(E51,1,"actual/360","simple","annual",I47)</f>
+        <f>_xll.qlBondDirtyPriceFromYield(F51,1,"actual/360","simple","annual",I47)</f>
         <v>2.9916897506925206</v>
       </c>
     </row>
@@ -1119,7 +1101,7 @@
         <v>PASS</v>
       </c>
       <c r="E32">
-        <f>_xll.qlBondBpsFromYield(E51,1,"actual/360","simple","annual",I47)</f>
+        <f>_xll.qlBondBpsFromYield(F51,1,"actual/360","simple","annual",I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -1135,7 +1117,7 @@
         <v>FAIL</v>
       </c>
       <c r="E33">
-        <f>_xll.qlBondYieldFromCleanPrice(E51,1,"actual/360","simple","annual",I47,0.0000000001,100,0.05)</f>
+        <f>_xll.qlBondYieldFromCleanPrice(F51,1,"actual/360","simple","annual",I47,0.0000000001,100,0.05)</f>
         <v>720</v>
       </c>
     </row>
@@ -1151,7 +1133,7 @@
         <v>FAIL</v>
       </c>
       <c r="E34">
-        <f>_xll.qlBondDurationFromYield(E51,1,"actual/360","simple","annual","modified",I47)</f>
+        <f>_xll.qlBondDurationFromYield(F51,1,"actual/360","simple","annual","modified",I47)</f>
         <v>2.7700831024930748E-3</v>
       </c>
     </row>
@@ -1167,7 +1149,7 @@
         <v>FAIL</v>
       </c>
       <c r="E35">
-        <f>_xll.qlBondConvexityFromYield(E51,1,"actual/360","simple","annual",I47)</f>
+        <f>_xll.qlBondConvexityFromYield(F51,1,"actual/360","simple","annual",I47)</f>
         <v>1.5346720789435321E-5</v>
       </c>
     </row>
@@ -1183,7 +1165,7 @@
         <v>FAIL</v>
       </c>
       <c r="E36">
-        <f>_xll.qlBondCleanPriceFromZSpread(E51,G27,1,"actual/360","simple","annual",I47)</f>
+        <f>_xll.qlBondCleanPriceFromZSpread(F51,G27,1,"actual/360","simple","annual",I47)</f>
         <v>2.9834254143646408</v>
       </c>
     </row>
@@ -1199,7 +1181,7 @@
         <v>FAIL</v>
       </c>
       <c r="E37">
-        <f>_xll.qlBondZSpreadFromCleanPrice(E51,1,G27,"actual/360","simple","annual",I47,0.0000000001,100,0)</f>
+        <f>_xll.qlBondZSpreadFromCleanPrice(F51,1,G27,"actual/360","simple","annual",I47,0.0000000001,100,0)</f>
         <v>718.99999999999989</v>
       </c>
     </row>
@@ -1215,7 +1197,7 @@
         <v>PASS</v>
       </c>
       <c r="E38">
-        <f>_xll.qlBondCleanPrice(E51)</f>
+        <f>_xll.qlBondCleanPrice(F51)</f>
         <v>0</v>
       </c>
     </row>
@@ -1231,7 +1213,7 @@
         <v>FAIL</v>
       </c>
       <c r="E39" t="str">
-        <f>_xll.qlBondDescription(E51)</f>
+        <f>_xll.qlBondDescription(F51)</f>
         <v>abc</v>
       </c>
     </row>
@@ -1247,7 +1229,7 @@
         <v>FAIL</v>
       </c>
       <c r="E40" t="str">
-        <f>_xll.qlBondCurrency(E51)</f>
+        <f>_xll.qlBondCurrency(F51)</f>
         <v>EUR</v>
       </c>
     </row>
@@ -1263,7 +1245,7 @@
         <v>FAIL</v>
       </c>
       <c r="E41">
-        <f>_xll.qlBondRedemptionAmount(E51)</f>
+        <f>_xll.qlBondRedemptionAmount(F51)</f>
         <v>3</v>
       </c>
     </row>
@@ -1279,7 +1261,7 @@
         <v>FAIL</v>
       </c>
       <c r="E42">
-        <f>_xll.qlBondRedemptionDate(E51)</f>
+        <f>_xll.qlBondRedemptionDate(F51)</f>
         <v>42647</v>
       </c>
     </row>
@@ -1295,7 +1277,7 @@
         <v>FAIL</v>
       </c>
       <c r="E43" t="str">
-        <f>_xll.qlBondFlowAnalysis(E51,I47)</f>
+        <f>_xll.qlBondFlowAnalysis(F51,I47)</f>
         <v>Payment Date</v>
       </c>
     </row>
@@ -1339,20 +1321,24 @@
       <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="B46" t="s">
-        <v>64</v>
+      <c r="B46" t="b">
+        <v>0</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E46" t="str">
-        <f>_xll.qlFixedRateBond("bond01","abc","eur",2,100,G46,J46:J48,"actual/360","mf",100,I46,"target")</f>
-        <v>bond01#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E46" t="b">
+        <f>ISERROR(F46)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" t="str">
+        <f>_xll.qlFixedRateBond(,"abc","eur",2,100,G46,J46:J48,"actual/360","mf",100,I46,"target")</f>
+        <v>obj_00007#0003</v>
       </c>
       <c r="G46" t="str">
         <f>_xll.qlSchedule(,I46,I48,"1D","target","mf","mf","backward",TRUE)</f>
-        <v>obj_00006#0000</v>
+        <v>obj_00006#0002</v>
       </c>
       <c r="I46" s="4">
         <f>I45+1</f>
@@ -1363,26 +1349,30 @@
       </c>
       <c r="K46" t="str">
         <f>_xll.qlInterestRate(,1,"actual/360","simple","annual")</f>
-        <v>obj_00001#0000</v>
+        <v>obj_00004#0002</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="B47" t="s">
-        <v>65</v>
+      <c r="B47" t="b">
+        <v>0</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E47" t="str">
-        <f>_xll.qlFixedRateBond2("bond02","abc","EUR",2,100,G46,K48,"mf",100,I46,"target")</f>
-        <v>bond02#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E47" t="b">
+        <f t="shared" ref="E47:E51" si="1">ISERROR(F47)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" t="str">
+        <f>_xll.qlFixedRateBond2(,"abc","EUR",2,100,G46,K48,"mf",100,I46,"target")</f>
+        <v>obj_00009#0003</v>
       </c>
       <c r="I47" s="4">
-        <f t="shared" ref="I47:I48" si="1">I46+1</f>
+        <f t="shared" ref="I47:I48" si="2">I46+1</f>
         <v>42646</v>
       </c>
       <c r="J47">
@@ -1390,30 +1380,34 @@
       </c>
       <c r="K47" t="str">
         <f>_xll.qlInterestRate(,2,"actual/360","simple","annual")</f>
-        <v>obj_00004#0000</v>
+        <v>obj_00001#0002</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
-      <c r="B48" t="s">
-        <v>66</v>
+      <c r="B48" t="b">
+        <v>0</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E48" t="str">
-        <f>_xll.qlFloatingRateBond("bond03","abc","eur",2,"mf",100,G46,2,FALSE,"actual/360",1,1,G48,0,2,100,+I46)</f>
-        <v>bond03#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E48" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48" t="str">
+        <f>_xll.qlFloatingRateBond(,"abc","eur",2,"mf",100,G46,2,FALSE,"actual/360",1,1,G48,0,2,100,+I46)</f>
+        <v>obj_00008#0003</v>
       </c>
       <c r="G48" t="str">
         <f>_xll.qlIborIndex(,"euribor","1d",2,"eur","target","mf",TRUE,"actual/360")</f>
-        <v>obj_00002#0000</v>
+        <v>obj_00000#0002</v>
       </c>
       <c r="I48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42647</v>
       </c>
       <c r="J48">
@@ -1421,63 +1415,75 @@
       </c>
       <c r="K48" t="str">
         <f>_xll.qlInterestRate(,3,"actual/360","simple","annual")</f>
-        <v>obj_00000#0000</v>
+        <v>obj_00003#0002</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
-        <v>67</v>
+      <c r="B49" t="b">
+        <v>0</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E49" t="str">
-        <f>_xll.qlCmsRateBond("bond04","abc","eur",2,"mf",100,+G46,2,FALSE,"actual/360",1,1,G49,0,2,100,I46)</f>
-        <v>bond04#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E49" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49" t="str">
+        <f>_xll.qlCmsRateBond(,"abc","eur",2,"mf",100,+G46,2,FALSE,"actual/360",1,1,G49,0,2,100,I46)</f>
+        <v>obj_0000d#0003</v>
       </c>
       <c r="G49" t="str">
         <f>_xll.qlSwapIndex(,"euribor","1d",2,"eur","target","1d","mf","actual/360",G48)</f>
-        <v>obj_00005#0000</v>
+        <v>obj_00005#0002</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
-      <c r="B50" t="s">
-        <v>68</v>
+      <c r="B50" t="b">
+        <v>0</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E50" t="str">
-        <f>_xll.qlZeroCouponBond("bond05","abc","eur",2,"target",100,I48,"mf",100,+I46)</f>
-        <v>bond05#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F50" t="str">
+        <f>_xll.qlZeroCouponBond(,"abc","eur",2,"target",100,I48,"mf",100,+I46)</f>
+        <v>obj_0000a#0003</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" t="s">
-        <v>69</v>
+      <c r="B51" t="b">
+        <v>0</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E51" t="str">
-        <f>_xll.qlBond("bond06","abc","eur",2,"target",100,I48,I45,G51)</f>
-        <v>bond06#0000</v>
+        <v>PASS</v>
+      </c>
+      <c r="E51" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F51" t="str">
+        <f>_xll.qlBond(,"abc","eur",2,"target",100,I48,I45,G51)</f>
+        <v>obj_0000c#0003</v>
       </c>
       <c r="G51" t="str">
         <f>_xll.qlLeg(,J46:J48,I46:I48)</f>
-        <v>obj_00009#0000</v>
+        <v>obj_0000b#0002</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1492,7 +1498,7 @@
         <v>ERROR</v>
       </c>
       <c r="E52" t="e">
-        <f>_xll.qlBondAlive(E51,I47)</f>
+        <f>_xll.qlBondAlive(F51,I47)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1501,14 +1507,14 @@
         <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E53" t="str">
-        <f>_xll.qlBondMaturityLookup(E51,I47)</f>
+        <f>_xll.qlBondMaturityLookup(F51,I47)</f>
         <v/>
       </c>
     </row>
@@ -1517,15 +1523,15 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
       <c r="E54" t="str">
-        <f>_xll.qlBondMaturitySort(E51)</f>
-        <v>bond06</v>
+        <f>_xll.qlBondMaturitySort(F51)</f>
+        <v>obj_0000c</v>
       </c>
     </row>
   </sheetData>

</xml_diff>